<commit_message>
update to relhum data process
</commit_message>
<xml_diff>
--- a/data_process/2d_1d/processed_data/relhum_std_ratios.xlsx
+++ b/data_process/2d_1d/processed_data/relhum_std_ratios.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Uninsulated" sheetId="1" r:id="rId1"/>
+    <sheet name="Insulated" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>location</t>
   </si>
@@ -70,6 +71,27 @@
   </si>
   <si>
     <t>0.3715</t>
+  </si>
+  <si>
+    <t>Brick: Dresden ZD - Mortar: High Cement Ratio - Insulation: Calcium Silicate</t>
+  </si>
+  <si>
+    <t>Brick: Dresden ZP - Mortar: High Cement Ratio - Insulation: Calcium Silicate</t>
+  </si>
+  <si>
+    <t>Brick: Potsdam - Mortar: High Cement Ratio - Insulation: Calcium Silicate</t>
+  </si>
+  <si>
+    <t>Brick: Dresden ZD - Mortar: Low Cement Ratio - Insulation: Calcium Silicate</t>
+  </si>
+  <si>
+    <t>Brick: Dresden ZP - Mortar: Low Cement Ratio - Insulation: Calcium Silicate</t>
+  </si>
+  <si>
+    <t>Brick: Potsdam - Mortar: Low Cement Ratio - Insulation: Calcium Silicate</t>
+  </si>
+  <si>
+    <t>0.4895</t>
   </si>
 </sst>
 </file>
@@ -133,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -141,14 +163,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -455,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,369 +495,369 @@
     <col min="3" max="9" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5">
-        <v>4.8640970029045057E-2</v>
-      </c>
-      <c r="D2" s="5">
-        <v>5.2281115634869299E-2</v>
-      </c>
-      <c r="E2" s="5">
-        <v>5.3080171987367301E-2</v>
-      </c>
-      <c r="F2" s="5">
-        <v>5.3422624709866452E-2</v>
-      </c>
-      <c r="G2" s="5">
-        <v>4.893268901487767E-2</v>
-      </c>
-      <c r="H2" s="5">
-        <v>4.8894638712377772E-2</v>
-      </c>
-      <c r="I2" s="5">
-        <v>5.0074198089874823E-2</v>
+      <c r="C2" s="4">
+        <v>1.8708065395786559E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.6970434914957571E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2.0356911837449108E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2.0585213652448541E-2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1.735093793995662E-2</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2.024276092994939E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>2.0014459114949961E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5">
-        <v>7.0976497596489219E-2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>7.5377649252311552E-2</v>
-      </c>
-      <c r="E3" s="5">
-        <v>6.1070735512347332E-2</v>
-      </c>
-      <c r="F3" s="5">
-        <v>5.962482401735094E-2</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.1201628552946996</v>
-      </c>
-      <c r="H3" s="5">
-        <v>9.0103116319774745E-2</v>
-      </c>
-      <c r="I3" s="5">
-        <v>8.6754689699783116E-2</v>
+      <c r="C3" s="4">
+        <v>1.9570538919117739E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.468741676496328E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.0737414862448161E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2.1003766979947491E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.7084585822457289E-2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2.1574521517446061E-2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2.1916974239945208E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5">
-        <v>0.1251411032051038</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.14432479738213921</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.1397587610821506</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.14002511319964989</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.1186788934972033</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.1151021650622122</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.1130854990297173</v>
+      <c r="C4" s="4">
+        <v>2.2202351508694491E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.8454396712453861E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.0280811232449299E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.9633956089950919E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2.024276092994939E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.940565427495149E-2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1.9139302157452149E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5">
-        <v>0.13382291389216541</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.13606788173965981</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.17008485217457481</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.16749743160458119</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.11042197785472389</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.11205814086221989</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.1112590845097219</v>
+      <c r="C5" s="4">
+        <v>1.8308537219537561E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.9786157299950539E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.2061945892469851E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.2937102849967659E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.3819489364940449E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.9633956089950919E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1.932955366995168E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.1349263726646627</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.1757543472470606</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.34237662189414408</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.1958068566645105</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.13808454777215479</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.1453521555496366</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.13389901449716529</v>
+      <c r="C6" s="4">
+        <v>2.181550676661213E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.434496404246414E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.0226399299874436E-3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.87587991324531E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.1155968189947111E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2.2335527567444158E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.3971690574940072E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5">
-        <v>0.1467727001762997</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.16506221224458731</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.19093641794452271</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.19291503367451771</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.1430691373996423</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.1654427152695864</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.1646817092195883</v>
+      <c r="C7" s="4">
+        <v>1.9741765280367311E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.522012099996195E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.1491191354971271E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.111068832997222E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1.8796849434953009E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.4915718579962709E-2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.4535215554963661E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
-        <v>0.1908095836028563</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.32571058939918568</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.41151402153647121</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.49720330276625702</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.1459609603896351</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.1515163045546212</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0.1448575016171379</v>
+      <c r="C8" s="4">
+        <v>2.3312151998275049E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2.492294813743769E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>3.5006278299912492E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3.3027662569917432E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5">
-        <v>0.1105805207818069</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.28457821239678849</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.24751721776188121</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.26281343936684298</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.1412427228796469</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.1621323389520947</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0.16125718199459679</v>
+      <c r="C9" s="4">
+        <v>2.712352396534886E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5.0987405349872533E-3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.712263612495719E-3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1.693238461245767E-2</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1.221414710246947E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.229024770746927E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5">
-        <v>0.96685184480549957</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.90681480917773294</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.98314371599254213</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0.9370267493626574</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0.93969027053765075</v>
+      <c r="C10" s="4">
+        <v>8.4535088720621987E-3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1.48396179749629E-2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1.826414519995434E-3</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1.4459114949963851E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5">
-        <v>0.86814936012074628</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.87732582474030674</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.90335223165024159</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.84578212396788555</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.92709562041018223</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.97606635972755984</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.90582550131273543</v>
+      <c r="C11" s="4">
+        <v>4.6611620562383473E-3</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.8073893687454819E-2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1.5752825234960618E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2.2069175449944831E-2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1.434496404246414E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5">
-        <v>0.98144413581421308</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.99520566188501203</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.9993531448575016</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.98337201780754158</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.95456793881511359</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0.94383775351014043</v>
+      <c r="C12" s="4">
+        <v>3.5703867179077411E-3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3.04402419999239E-4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.141509074997146E-4</v>
+      </c>
+      <c r="F12" s="4">
+        <v>6.8490544499828776E-4</v>
+      </c>
+      <c r="G12" s="4">
+        <v>3.0820745024922949E-3</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1.826414519995434E-3</v>
+      </c>
+      <c r="I12" s="4">
+        <v>4.6040866024884899E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5">
-        <v>0.98368910366170748</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.99676572428750809</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.99980974848750048</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.98790000380503029</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.9537688824626156</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.93607549180015981</v>
+      <c r="C13" s="4">
+        <v>4.8450718516545536E-3</v>
+      </c>
+      <c r="D13" s="4">
+        <v>9.5125756249762189E-4</v>
+      </c>
+      <c r="E13" s="4">
+        <v>4.5660362999885851E-4</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.217609679996956E-3</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3.19622540999201E-3</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2.0927666374947682E-3</v>
+      </c>
+      <c r="I13" s="4">
+        <v>3.3864769224915339E-3</v>
       </c>
     </row>
   </sheetData>
@@ -840,4 +871,452 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="9" width="19.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.3545907689966139E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.434496404246414E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.7465088847456341E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1.6475780982458811E-2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1.263270042996842E-2</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1.5182070697462051E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1.5448422814961379E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.1801935492053829E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.1947794984970129E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.16814428674708E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.1491191354971271E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.1871694379970319E-2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.2138046497469661E-2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.2138046497469661E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.195502454244511E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.146037060994635E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.3058483314942351E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2.2145276054944641E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1.8606597922453481E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.834024580495415E-2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1.7312887637456718E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.9234427913701911E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.7959742779955101E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.5067919789962331E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.529622160496176E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.0851565769947868E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2.0737414862448161E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2.0585213652448541E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.0521796481615361E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.0425782884973939E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.974810699745063E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.0958487119972601E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.0128610022449679E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2.024276092994939E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1.7503139149956239E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2.0122268305366359E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.183364407747042E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.156729195997108E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.122483923747194E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2.0927666374947682E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.9938358509950151E-2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.9519805182451201E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.1588092792004363E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2.8537726874928661E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2.929873292492675E-3</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2.1232068794946921E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2.1840873634945399E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.7807541569955478E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3.285009449158454E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2.081351546744797E-2</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1.495376888246262E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.48396179749629E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.454244511243864E-3</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.7562878124881086E-3</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1.902515124995244E-3</v>
+      </c>
+      <c r="I11" s="4">
+        <v>3.4625775274913441E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.1383382164554871E-2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.487766827746281E-2</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1.4801567672463E-2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1.388836041246528E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>